<commit_message>
Error checking for open file works.
</commit_message>
<xml_diff>
--- a/aa-archive/books_spreadsheet_out copy.xlsx
+++ b/aa-archive/books_spreadsheet_out copy.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C25F9CC-A348-451D-A39B-C457760A65C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4348FA3-239D-4AAC-9A1D-DF7334429FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Book Hoard" sheetId="2" r:id="rId2"/>
+    <sheet name="Book Hoard" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="GLS" localSheetId="1">'Book Hoard'!$A$1:$AV$1</definedName>
+    <definedName name="GLS" localSheetId="0">'Book Hoard'!$A$1:$AV$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -41,6 +40,12 @@
     <t>weight</t>
   </si>
   <si>
+    <t>current_language</t>
+  </si>
+  <si>
+    <t>original_language</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -59,6 +64,9 @@
     <t>complexity_esoteric</t>
   </si>
   <si>
+    <t>fraction_complete</t>
+  </si>
+  <si>
     <t>market_value</t>
   </si>
   <si>
@@ -71,12 +79,6 @@
     <t>translator_full_name</t>
   </si>
   <si>
-    <t>current_language</t>
-  </si>
-  <si>
-    <t>original_language</t>
-  </si>
-  <si>
     <t>book_title_flavor</t>
   </si>
   <si>
@@ -93,9 +95,6 @@
   </si>
   <si>
     <t>number_extant_available_to_place</t>
-  </si>
-  <si>
-    <t>fraction_complete</t>
   </si>
   <si>
     <t>rarity_modifier</t>
@@ -191,9 +190,8 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -534,18 +532,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -559,29 +545,29 @@
     <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="137.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="48.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="36.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="142.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="24" style="2" customWidth="1"/>
-    <col min="23" max="23" width="34" style="2" customWidth="1"/>
-    <col min="24" max="24" width="19.28515625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="71.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="29.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="69.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="21.28515625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="32" style="3" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="3" customWidth="1"/>
     <col min="26" max="26" width="34.42578125" style="1" customWidth="1"/>
-    <col min="27" max="29" width="9.140625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="27" max="32" width="9.140625" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>